<commit_message>
BTD incremental backup 20230717
</commit_message>
<xml_diff>
--- a/Data_Files/BTD - Test Config Options.xlsx
+++ b/Data_Files/BTD - Test Config Options.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://haefele-my.sharepoint.com/personal/richard_varney_hafele_co_uk/Documents/Documents/Ranorex/RanorexStudio Projects/HUKBespokeTimberDrawers/Data_Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{5FCF2620-8DF3-4D0C-B47D-36B83AF28C4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{74713508-FB2D-4097-9CF8-2ED1DF9E82AC}"/>
+  <xr:revisionPtr revIDLastSave="86" documentId="13_ncr:1_{5FCF2620-8DF3-4D0C-B47D-36B83AF28C4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F7F42F67-5968-47C9-8A1F-146FB70B6D3D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="571" xr2:uid="{C6F55A37-2B61-455A-B735-6B3A9C9B662C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="571" activeTab="1" xr2:uid="{C6F55A37-2B61-455A-B735-6B3A9C9B662C}"/>
   </bookViews>
   <sheets>
     <sheet name="MasterData" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2782" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2782" uniqueCount="274">
   <si>
     <t>Amend Existing Quote</t>
   </si>
@@ -862,6 +862,12 @@
   <si>
     <t>IntHeight_mm</t>
   </si>
+  <si>
+    <t>Logo_Upload</t>
+  </si>
+  <si>
+    <t>C:\Users\HUK2146\OneDrive - Haefele SE &amp; Co KG\Documents\Ranorex\RanorexStudio Projects\HUKBespokeTimberDrawers\BTD_Logos\BTD_Logo.jpg</t>
+  </si>
 </sst>
 </file>
 
@@ -1609,10 +1615,10 @@
   </sheetPr>
   <dimension ref="A1:BJ88"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="AG1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="AK1" sqref="AK1"/>
-      <selection pane="bottomLeft" activeCell="J1" sqref="J1"/>
+      <selection pane="bottomLeft" activeCell="AI2" sqref="AI2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1648,7 +1654,8 @@
     <col min="31" max="31" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="116.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="46.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="35" width="46.42578125" style="1" customWidth="1"/>
+    <col min="34" max="34" width="46.42578125" style="1" customWidth="1"/>
+    <col min="35" max="35" width="116.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="17.5703125" style="14" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="19.5703125" style="14" bestFit="1" customWidth="1"/>
     <col min="38" max="39" width="17.5703125" style="14" customWidth="1"/>
@@ -1789,7 +1796,7 @@
         <v>236</v>
       </c>
       <c r="AI1" s="3" t="s">
-        <v>259</v>
+        <v>272</v>
       </c>
       <c r="AJ1" s="13" t="s">
         <v>54</v>
@@ -1876,15 +1883,15 @@
     <row r="2" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <f>Login!A2</f>
-        <v>30230</v>
+        <v>310077</v>
       </c>
       <c r="B2" s="1" t="str">
         <f>Login!B2</f>
-        <v>pingu</v>
+        <v>MYNEWPASSWORD123</v>
       </c>
       <c r="C2" s="22" t="str">
         <f>Login!C2</f>
-        <v>My account(30230)</v>
+        <v>My account(310077)</v>
       </c>
       <c r="F2" s="1" t="str">
         <f>Parametres!A2</f>
@@ -1984,7 +1991,7 @@
       </c>
       <c r="AF2" s="1" t="str">
         <f>Engraving!D2</f>
-        <v>C:\Users\hukit9999\Documents\Ranorex\RanorexStudio Projects\OneWeb-Ranorex\HUKWebTesting\BTD_Logos\BTD_Logo.jpg</v>
+        <v>C:\Users\HUK2146\OneDrive - Haefele SE &amp; Co KG\Documents\Ranorex\RanorexStudio Projects\HUKBespokeTimberDrawers\BTD_Logos\BTD_Logo.jpg</v>
       </c>
       <c r="AG2" s="1" t="str">
         <f>Engraving!C2</f>
@@ -2087,15 +2094,15 @@
     <row r="3" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <f>Login!A3</f>
-        <v>30230</v>
+        <v>310077</v>
       </c>
       <c r="B3" s="1" t="str">
         <f>Login!B3</f>
-        <v>pingu</v>
+        <v>MYNEWPASSWORD123</v>
       </c>
       <c r="C3" s="22" t="str">
         <f>Login!C3</f>
-        <v>My account(30230)</v>
+        <v>My account(310077)</v>
       </c>
       <c r="F3" s="1" t="str">
         <f>Parametres!A3</f>
@@ -2219,7 +2226,7 @@
       </c>
       <c r="AN3" s="80">
         <f ca="1">'Delivery Address'!A3</f>
-        <v>45110.517463310185</v>
+        <v>45124.458862037034</v>
       </c>
       <c r="AO3" s="1" t="s">
         <v>39</v>
@@ -2266,15 +2273,15 @@
     <row r="4" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <f>Login!A4</f>
-        <v>30230</v>
+        <v>310077</v>
       </c>
       <c r="B4" s="1" t="str">
         <f>Login!B4</f>
-        <v>pingu</v>
+        <v>MYNEWPASSWORD123</v>
       </c>
       <c r="C4" s="22" t="str">
         <f>Login!C4</f>
-        <v>My account(30230)</v>
+        <v>My account(310077)</v>
       </c>
       <c r="F4" s="1" t="str">
         <f>Parametres!A4</f>
@@ -2398,7 +2405,7 @@
       </c>
       <c r="AN4" s="80">
         <f ca="1">'Delivery Address'!A4</f>
-        <v>45110.517463310185</v>
+        <v>45124.458862037034</v>
       </c>
       <c r="AO4" s="1" t="s">
         <v>43</v>
@@ -2569,7 +2576,7 @@
       </c>
       <c r="AN5" s="80">
         <f ca="1">'Delivery Address'!A5</f>
-        <v>45110.517463310185</v>
+        <v>45124.458862037034</v>
       </c>
       <c r="AQ5" s="1">
         <f>'Delivery Address'!B5</f>
@@ -2595,15 +2602,15 @@
     <row r="6" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f>Login!A6</f>
-        <v>30230</v>
+        <v>310077</v>
       </c>
       <c r="B6" s="1" t="str">
         <f>Login!B6</f>
-        <v>pingu</v>
+        <v>MYNEWPASSWORD123</v>
       </c>
       <c r="C6" s="22" t="str">
         <f>Login!C6</f>
-        <v>My account(30230)</v>
+        <v>My account(310077)</v>
       </c>
       <c r="F6" s="1" t="str">
         <f>Parametres!A6</f>
@@ -2719,7 +2726,7 @@
       </c>
       <c r="AN6" s="80">
         <f ca="1">'Delivery Address'!A6</f>
-        <v>45110.517463310185</v>
+        <v>45124.458862037034</v>
       </c>
       <c r="AQ6" s="1">
         <f>'Delivery Address'!B6</f>
@@ -2745,15 +2752,15 @@
     <row r="7" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <f>Login!A7</f>
-        <v>30230</v>
+        <v>310077</v>
       </c>
       <c r="B7" s="1" t="str">
         <f>Login!B7</f>
-        <v>pingu</v>
+        <v>MYNEWPASSWORD123</v>
       </c>
       <c r="C7" s="22" t="str">
         <f>Login!C7</f>
-        <v>My account(30230)</v>
+        <v>My account(310077)</v>
       </c>
       <c r="F7" s="1" t="str">
         <f>Parametres!A7</f>
@@ -2869,7 +2876,7 @@
       </c>
       <c r="AN7" s="80">
         <f ca="1">'Delivery Address'!A7</f>
-        <v>45110.517463310185</v>
+        <v>45124.458862037034</v>
       </c>
       <c r="AQ7" s="1">
         <f>'Delivery Address'!B7</f>
@@ -2895,15 +2902,15 @@
     <row r="8" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <f>Login!A8</f>
-        <v>30230</v>
+        <v>310077</v>
       </c>
       <c r="B8" s="1" t="str">
         <f>Login!B8</f>
-        <v>pingu</v>
+        <v>MYNEWPASSWORD123</v>
       </c>
       <c r="C8" s="22" t="str">
         <f>Login!C8</f>
-        <v>My account(30230)</v>
+        <v>My account(310077)</v>
       </c>
       <c r="F8" s="1" t="str">
         <f>Parametres!A8</f>
@@ -3019,7 +3026,7 @@
       </c>
       <c r="AN8" s="80">
         <f ca="1">'Delivery Address'!A8</f>
-        <v>45110.517463310185</v>
+        <v>45124.458862037034</v>
       </c>
       <c r="AQ8" s="1">
         <f>'Delivery Address'!B8</f>
@@ -3045,15 +3052,15 @@
     <row r="9" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <f>Login!A9</f>
-        <v>30230</v>
+        <v>310077</v>
       </c>
       <c r="B9" s="1" t="str">
         <f>Login!B9</f>
-        <v>pingu</v>
+        <v>MYNEWPASSWORD123</v>
       </c>
       <c r="C9" s="22" t="str">
         <f>Login!C9</f>
-        <v>My account(30230)</v>
+        <v>My account(310077)</v>
       </c>
       <c r="F9" s="1" t="str">
         <f>Parametres!A9</f>
@@ -3169,7 +3176,7 @@
       </c>
       <c r="AN9" s="80">
         <f ca="1">'Delivery Address'!A9</f>
-        <v>45110.517463310185</v>
+        <v>45124.458862037034</v>
       </c>
       <c r="AQ9" s="1">
         <f>'Delivery Address'!B9</f>
@@ -3195,15 +3202,15 @@
     <row r="10" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <f>Login!A10</f>
-        <v>30230</v>
+        <v>310077</v>
       </c>
       <c r="B10" s="1" t="str">
         <f>Login!B10</f>
-        <v>pingu</v>
+        <v>MYNEWPASSWORD123</v>
       </c>
       <c r="C10" s="22" t="str">
         <f>Login!C10</f>
-        <v>My account(30230)</v>
+        <v>My account(310077)</v>
       </c>
       <c r="F10" s="1" t="str">
         <f>Parametres!A10</f>
@@ -3319,7 +3326,7 @@
       </c>
       <c r="AN10" s="80">
         <f ca="1">'Delivery Address'!A10</f>
-        <v>45110.517463310185</v>
+        <v>45124.458862037034</v>
       </c>
       <c r="AQ10" s="1">
         <f>'Delivery Address'!B10</f>
@@ -3345,15 +3352,15 @@
     <row r="11" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <f>Login!A11</f>
-        <v>30230</v>
+        <v>310077</v>
       </c>
       <c r="B11" s="1" t="str">
         <f>Login!B11</f>
-        <v>pingu</v>
+        <v>MYNEWPASSWORD123</v>
       </c>
       <c r="C11" s="22" t="str">
         <f>Login!C11</f>
-        <v>My account(30230)</v>
+        <v>My account(310077)</v>
       </c>
       <c r="F11" s="1" t="str">
         <f>Parametres!A11</f>
@@ -3469,7 +3476,7 @@
       </c>
       <c r="AN11" s="80">
         <f ca="1">'Delivery Address'!A11</f>
-        <v>45110.517463310185</v>
+        <v>45124.458862037034</v>
       </c>
       <c r="AQ11" s="1">
         <f>'Delivery Address'!B11</f>
@@ -3495,15 +3502,15 @@
     <row r="12" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <f>Login!A12</f>
-        <v>30230</v>
+        <v>310077</v>
       </c>
       <c r="B12" s="1" t="str">
         <f>Login!B12</f>
-        <v>pingu</v>
+        <v>MYNEWPASSWORD123</v>
       </c>
       <c r="C12" s="22" t="str">
         <f>Login!C12</f>
-        <v>My account(30230)</v>
+        <v>My account(310077)</v>
       </c>
       <c r="F12" s="1" t="str">
         <f>Parametres!A12</f>
@@ -3619,7 +3626,7 @@
       </c>
       <c r="AN12" s="80">
         <f ca="1">'Delivery Address'!A12</f>
-        <v>45110.517463310185</v>
+        <v>45124.458862037034</v>
       </c>
       <c r="AQ12" s="1">
         <f>'Delivery Address'!B12</f>
@@ -3645,15 +3652,15 @@
     <row r="13" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <f>Login!A13</f>
-        <v>30230</v>
+        <v>310077</v>
       </c>
       <c r="B13" s="1" t="str">
         <f>Login!B13</f>
-        <v>pingu</v>
+        <v>MYNEWPASSWORD123</v>
       </c>
       <c r="C13" s="22" t="str">
         <f>Login!C13</f>
-        <v>My account(30230)</v>
+        <v>My account(310077)</v>
       </c>
       <c r="F13" s="1" t="str">
         <f>Parametres!A13</f>
@@ -3769,7 +3776,7 @@
       </c>
       <c r="AN13" s="80">
         <f ca="1">'Delivery Address'!A13</f>
-        <v>45110.517463310185</v>
+        <v>45124.458862037034</v>
       </c>
       <c r="AQ13" s="1">
         <f>'Delivery Address'!B13</f>
@@ -3795,15 +3802,15 @@
     <row r="14" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <f>Login!A14</f>
-        <v>30230</v>
+        <v>310077</v>
       </c>
       <c r="B14" s="1" t="str">
         <f>Login!B14</f>
-        <v>pingu</v>
+        <v>MYNEWPASSWORD123</v>
       </c>
       <c r="C14" s="22" t="str">
         <f>Login!C14</f>
-        <v>My account(30230)</v>
+        <v>My account(310077)</v>
       </c>
       <c r="F14" s="1" t="str">
         <f>Parametres!A14</f>
@@ -3919,7 +3926,7 @@
       </c>
       <c r="AN14" s="80">
         <f ca="1">'Delivery Address'!A14</f>
-        <v>45110.517463310185</v>
+        <v>45124.458862037034</v>
       </c>
       <c r="AQ14" s="1">
         <f>'Delivery Address'!B14</f>
@@ -4069,7 +4076,7 @@
       </c>
       <c r="AN15" s="80">
         <f ca="1">'Delivery Address'!A15</f>
-        <v>45110.517463310185</v>
+        <v>45124.458862037034</v>
       </c>
       <c r="AQ15" s="1">
         <f>'Delivery Address'!B15</f>
@@ -4219,7 +4226,7 @@
       </c>
       <c r="AN16" s="80">
         <f ca="1">'Delivery Address'!A16</f>
-        <v>45110.517463310185</v>
+        <v>45124.458862037034</v>
       </c>
       <c r="AO16" s="1" t="str">
         <f>'Delivery Contact'!A16</f>
@@ -18534,9 +18541,9 @@
   </sheetPr>
   <dimension ref="A1:E88"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomLeft" activeCell="A14" sqref="A14:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18567,39 +18574,39 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="19">
-        <v>30230</v>
+        <v>310077</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>49</v>
+        <v>264</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>57</v>
+        <v>265</v>
       </c>
       <c r="D2" s="20"/>
       <c r="E2" s="20"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="19">
-        <v>30230</v>
+        <v>310077</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>49</v>
+        <v>264</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>57</v>
+        <v>265</v>
       </c>
       <c r="D3" s="20"/>
       <c r="E3" s="20"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="19">
-        <v>30230</v>
+        <v>310077</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>49</v>
+        <v>264</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>57</v>
+        <v>265</v>
       </c>
       <c r="D4" s="20"/>
       <c r="E4" s="20"/>
@@ -18619,117 +18626,117 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="19">
-        <v>30230</v>
+        <v>310077</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>49</v>
+        <v>264</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>57</v>
+        <v>265</v>
       </c>
       <c r="D6" s="20"/>
       <c r="E6" s="20"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="19">
-        <v>30230</v>
+        <v>310077</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>49</v>
+        <v>264</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>57</v>
+        <v>265</v>
       </c>
       <c r="D7" s="20"/>
       <c r="E7" s="20"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="19">
-        <v>30230</v>
+        <v>310077</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>49</v>
+        <v>264</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>57</v>
+        <v>265</v>
       </c>
       <c r="D8" s="20"/>
       <c r="E8" s="20"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="19">
-        <v>30230</v>
+        <v>310077</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>49</v>
+        <v>264</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>57</v>
+        <v>265</v>
       </c>
       <c r="D9" s="20"/>
       <c r="E9" s="20"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="19">
-        <v>30230</v>
+        <v>310077</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>49</v>
+        <v>264</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>57</v>
+        <v>265</v>
       </c>
       <c r="D10" s="20"/>
       <c r="E10" s="20"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="19">
-        <v>30230</v>
+        <v>310077</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>49</v>
+        <v>264</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>57</v>
+        <v>265</v>
       </c>
       <c r="D11" s="20"/>
       <c r="E11" s="20"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="19">
-        <v>30230</v>
+        <v>310077</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>49</v>
+        <v>264</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>57</v>
+        <v>265</v>
       </c>
       <c r="D12" s="20"/>
       <c r="E12" s="20"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="19">
-        <v>30230</v>
+        <v>310077</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>49</v>
+        <v>264</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>57</v>
+        <v>265</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="20"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="19">
-        <v>30230</v>
+        <v>310077</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>49</v>
+        <v>264</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>57</v>
+        <v>265</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="20"/>
@@ -26561,7 +26568,7 @@
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomLeft" activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26569,7 +26576,7 @@
     <col min="1" max="1" width="30.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="116.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="138.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -26597,7 +26604,7 @@
         <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>258</v>
+        <v>273</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -26611,7 +26618,7 @@
         <v>27</v>
       </c>
       <c r="D3" t="s">
-        <v>258</v>
+        <v>273</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -26625,7 +26632,7 @@
         <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>258</v>
+        <v>273</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -26639,7 +26646,7 @@
         <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>258</v>
+        <v>273</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -26653,7 +26660,7 @@
         <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>258</v>
+        <v>273</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -26667,7 +26674,7 @@
         <v>27</v>
       </c>
       <c r="D7" t="s">
-        <v>258</v>
+        <v>273</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -26681,7 +26688,7 @@
         <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>258</v>
+        <v>273</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -26695,7 +26702,7 @@
         <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>258</v>
+        <v>273</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -26709,7 +26716,7 @@
         <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>258</v>
+        <v>273</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -26723,7 +26730,7 @@
         <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>258</v>
+        <v>273</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -26737,7 +26744,7 @@
         <v>27</v>
       </c>
       <c r="D12" t="s">
-        <v>258</v>
+        <v>273</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -26751,7 +26758,7 @@
         <v>27</v>
       </c>
       <c r="D13" t="s">
-        <v>258</v>
+        <v>273</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -26765,7 +26772,7 @@
         <v>27</v>
       </c>
       <c r="D14" t="s">
-        <v>258</v>
+        <v>273</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -26779,7 +26786,7 @@
         <v>27</v>
       </c>
       <c r="D15" t="s">
-        <v>258</v>
+        <v>273</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -26793,7 +26800,7 @@
         <v>27</v>
       </c>
       <c r="D16" t="s">
-        <v>258</v>
+        <v>273</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -26807,7 +26814,7 @@
         <v>27</v>
       </c>
       <c r="D17" t="s">
-        <v>258</v>
+        <v>273</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -26821,7 +26828,7 @@
         <v>27</v>
       </c>
       <c r="D18" t="s">
-        <v>258</v>
+        <v>273</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -26835,7 +26842,7 @@
         <v>27</v>
       </c>
       <c r="D19" t="s">
-        <v>258</v>
+        <v>273</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -26849,7 +26856,7 @@
         <v>27</v>
       </c>
       <c r="D20" t="s">
-        <v>258</v>
+        <v>273</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -26863,7 +26870,7 @@
         <v>27</v>
       </c>
       <c r="D21" t="s">
-        <v>258</v>
+        <v>273</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -26877,7 +26884,7 @@
         <v>27</v>
       </c>
       <c r="D22" t="s">
-        <v>258</v>
+        <v>273</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -26891,7 +26898,7 @@
         <v>27</v>
       </c>
       <c r="D23" t="s">
-        <v>258</v>
+        <v>273</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -26905,7 +26912,7 @@
         <v>27</v>
       </c>
       <c r="D24" t="s">
-        <v>258</v>
+        <v>273</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -26919,7 +26926,7 @@
         <v>27</v>
       </c>
       <c r="D25" t="s">
-        <v>258</v>
+        <v>273</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -26933,7 +26940,7 @@
         <v>27</v>
       </c>
       <c r="D26" t="s">
-        <v>258</v>
+        <v>273</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -26947,7 +26954,7 @@
         <v>27</v>
       </c>
       <c r="D27" t="s">
-        <v>258</v>
+        <v>273</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -26961,7 +26968,7 @@
         <v>27</v>
       </c>
       <c r="D28" t="s">
-        <v>258</v>
+        <v>273</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -26975,7 +26982,7 @@
         <v>27</v>
       </c>
       <c r="D29" t="s">
-        <v>258</v>
+        <v>273</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -26989,7 +26996,7 @@
         <v>27</v>
       </c>
       <c r="D30" t="s">
-        <v>258</v>
+        <v>273</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -27003,7 +27010,7 @@
         <v>27</v>
       </c>
       <c r="D31" t="s">
-        <v>258</v>
+        <v>273</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -27017,7 +27024,7 @@
         <v>27</v>
       </c>
       <c r="D32" t="s">
-        <v>258</v>
+        <v>273</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -27031,7 +27038,7 @@
         <v>27</v>
       </c>
       <c r="D33" t="s">
-        <v>258</v>
+        <v>273</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -27045,7 +27052,7 @@
         <v>27</v>
       </c>
       <c r="D34" t="s">
-        <v>258</v>
+        <v>273</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -27059,7 +27066,7 @@
         <v>27</v>
       </c>
       <c r="D35" t="s">
-        <v>258</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -28687,7 +28694,7 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="77">
         <f t="shared" ref="A3:A19" ca="1" si="0">(NOW())</f>
-        <v>45110.517463310185</v>
+        <v>45124.458862037034</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>103</v>
@@ -28711,7 +28718,7 @@
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="77">
         <f t="shared" ca="1" si="0"/>
-        <v>45110.517463310185</v>
+        <v>45124.458862037034</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>101</v>
@@ -28735,7 +28742,7 @@
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="77">
         <f t="shared" ca="1" si="0"/>
-        <v>45110.517463310185</v>
+        <v>45124.458862037034</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
@@ -28759,67 +28766,67 @@
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="77">
         <f t="shared" ca="1" si="0"/>
-        <v>45110.517463310185</v>
+        <v>45124.458862037034</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="77">
         <f t="shared" ca="1" si="0"/>
-        <v>45110.517463310185</v>
+        <v>45124.458862037034</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="77">
         <f t="shared" ca="1" si="0"/>
-        <v>45110.517463310185</v>
+        <v>45124.458862037034</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="77">
         <f t="shared" ca="1" si="0"/>
-        <v>45110.517463310185</v>
+        <v>45124.458862037034</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="77">
         <f t="shared" ca="1" si="0"/>
-        <v>45110.517463310185</v>
+        <v>45124.458862037034</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="77">
         <f t="shared" ca="1" si="0"/>
-        <v>45110.517463310185</v>
+        <v>45124.458862037034</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="77">
         <f t="shared" ca="1" si="0"/>
-        <v>45110.517463310185</v>
+        <v>45124.458862037034</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="77">
         <f t="shared" ca="1" si="0"/>
-        <v>45110.517463310185</v>
+        <v>45124.458862037034</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="77">
         <f t="shared" ca="1" si="0"/>
-        <v>45110.517463310185</v>
+        <v>45124.458862037034</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="77">
         <f t="shared" ca="1" si="0"/>
-        <v>45110.517463310185</v>
+        <v>45124.458862037034</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="77">
         <f t="shared" ca="1" si="0"/>
-        <v>45110.517463310185</v>
+        <v>45124.458862037034</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>102</v>
@@ -28843,19 +28850,19 @@
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="77">
         <f t="shared" ca="1" si="0"/>
-        <v>45110.517463310185</v>
+        <v>45124.458862037034</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="77">
         <f t="shared" ca="1" si="0"/>
-        <v>45110.517463310185</v>
+        <v>45124.458862037034</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="77">
         <f t="shared" ca="1" si="0"/>
-        <v>45110.517463310185</v>
+        <v>45124.458862037034</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>